<commit_message>
add condition and comments
</commit_message>
<xml_diff>
--- a/inst/app/www/template.xlsx
+++ b/inst/app/www/template.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="3" r:id="rId1"/>
     <sheet name="NAME" sheetId="10" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.0" hidden="1">NAME!$G$8:$G$19</definedName>
-    <definedName name="_xlchart.1" hidden="1">NAME!$O$8:$O$19</definedName>
+    <definedName name="_xlchart.0" hidden="1">NAME!$G$11:$G$25</definedName>
+    <definedName name="_xlchart.1" hidden="1">NAME!$O$11:$O$25</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,8 +28,618 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Mickaël Canouil</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Date at which the experiment (Optical Density measures).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unique name or id to allow correction for operator in the analyses.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unique name for the project, i.e., a name allowing to group different experiments which should be analysed together.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The concentrations of insulin used to established the blank curve.
+Could use more or less points.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Optical Density measures.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Optical Density measures.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Mickaël Canouil</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Don't fill this column manually!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Don't fill this column manually!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Don't fill this column manually!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Don't fill this column manually!
+Please fill the name of the sheet instead!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Protocol has three steps, namely LYSAT, SN1 and SN2.
+Each steps should have the same number of samples (rows).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+'Reference' are experiments which will be used to define the basal insulin secretion, i.e., the threshold of insulin secreation is defined based on 'Reference'. 'Reference' are also 'Control' if no 'Control' are define.
+'Control' are experiments used to compare with 'Target'.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Labels used in the x-axis for figures.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Main treatment condition.
+This will be used in the analyses to ensure measurements are grouped and compared properly.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Optical Density measures.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Optical Density measures.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mickaël Canouil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not used in 'insane'.
+Only for 'interactive' reading when filling the template.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="37">
   <si>
     <t>OD2</t>
   </si>
@@ -41,18 +651,6 @@
   </si>
   <si>
     <t>Operator</t>
-  </si>
-  <si>
-    <t>16,7 mM Glc</t>
-  </si>
-  <si>
-    <t>16,7 mM Glc + IBMX</t>
-  </si>
-  <si>
-    <t>0,5 mM Glc</t>
-  </si>
-  <si>
-    <t>0,5 mM Glc + IBMX</t>
   </si>
   <si>
     <t>BLANK</t>
@@ -118,9 +716,6 @@
     <t>Glc</t>
   </si>
   <si>
-    <t>Glc + IBMX</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -132,12 +727,36 @@
   <si>
     <t>PROJECT_NAME</t>
   </si>
+  <si>
+    <t>16.7 mM Glc</t>
+  </si>
+  <si>
+    <t>0.5 mM Glc</t>
+  </si>
+  <si>
+    <t>16.7 mM Glc + A</t>
+  </si>
+  <si>
+    <t>Glc + A</t>
+  </si>
+  <si>
+    <t>16.7 mM Glc + B</t>
+  </si>
+  <si>
+    <t>Glc + B</t>
+  </si>
+  <si>
+    <t>0.5 mM Glc + A</t>
+  </si>
+  <si>
+    <t>0.5 mM Glc + B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +787,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +817,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,15 +860,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -227,12 +875,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1929,7 +2593,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>733424</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2252,12 +2916,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2268,243 +2930,243 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <f ca="1">TODAY()</f>
-        <v>43839</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="10">
+        <v>43892</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8">
         <v>0</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="4" t="e">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="13" t="e">
         <f t="shared" ref="H2:H7" si="0">AVERAGE(F2:G2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="M2" t="e">
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="M2" s="13" t="e">
         <f>INTERCEPT($I$3:$I$7,$J$3:$J$7)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N2" t="e">
+      <c r="N2" s="13" t="e">
         <f>SLOPE($I$3:$I$7,$J$3:$J$7)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B3" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B3" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C3" s="5" t="str">
+      <c r="C3" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="8">
         <v>3</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="4" t="e">
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I3" s="4" t="e">
+      <c r="I3" s="13" t="e">
         <f>LOG(H3-$H$2, 10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="13">
         <f>LOG(E3/23, 10)</f>
         <v>-0.88460658129793046</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B4" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B4" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C4" s="5" t="str">
+      <c r="C4" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="8">
         <v>9.74</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="4" t="e">
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I4" s="4" t="e">
+      <c r="I4" s="13" t="e">
         <f t="shared" ref="I4:I7" si="1">LOG(H4-$H$2, 10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="13">
         <f t="shared" ref="J4:J7" si="2">LOG(E4/23, 10)</f>
         <v>-0.37316887913897728</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B5" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B5" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C5" s="5" t="str">
+      <c r="C5" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10">
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8">
         <v>29.8</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="4" t="e">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I5" s="4" t="e">
+      <c r="I5" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="13">
         <f t="shared" si="2"/>
         <v>0.11248842805866237</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B6" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B6" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C6" s="5" t="str">
+      <c r="C6" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8">
         <v>104</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="4" t="e">
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I6" s="4" t="e">
+      <c r="I6" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="13">
         <f t="shared" si="2"/>
         <v>0.65530550328118731</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B7" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B7" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C7" s="5" t="str">
+      <c r="C7" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="8">
         <v>207</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="4" t="e">
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I7" s="4" t="e">
+      <c r="I7" s="13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="13">
         <f t="shared" si="2"/>
         <v>0.95424250943932487</v>
       </c>
@@ -2513,14 +3175,15 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2528,8 +3191,8 @@
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -2538,87 +3201,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="C1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>21</v>
+      <c r="N1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B2" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B2" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C2" s="2" t="str">
+      <c r="C2" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <f t="shared" ref="D2:D19" ca="1" si="0">RIGHT(CELL("nomfichier",A1),LEN(CELL("nomfichier",A1))-SEARCH("]",CELL("nomfichier",A1)))</f>
+      <c r="D2" s="16" t="str">
+        <f t="shared" ref="D2:D28" ca="1" si="0">RIGHT(CELL("nomfichier",A1),LEN(CELL("nomfichier",A1))-SEARCH("]",CELL("nomfichier",A1)))</f>
         <v>NAME</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4">
         <v>500</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="4">
         <f>50</f>
         <v>50</v>
       </c>
@@ -2627,46 +3290,46 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N2" s="1" t="e">
-        <f t="shared" ref="N2:N19" si="1">(L2/10^3 * M2)</f>
+        <f t="shared" ref="N2:N25" si="1">(L2/10^3 * M2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B3" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B3" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C3" s="2" t="str">
+      <c r="C3" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D3" s="1" t="str">
+      <c r="D3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4">
         <v>500</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="4">
         <f>50</f>
         <v>50</v>
       </c>
@@ -2681,40 +3344,40 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B4" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B4" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C4" s="2" t="str">
+      <c r="C4" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D4" s="1" t="str">
+      <c r="D4" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
         <v>500</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="4">
         <f>50</f>
         <v>50</v>
       </c>
@@ -2729,337 +3392,331 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B5" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B5" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C5" s="2" t="str">
+      <c r="C5" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D5" s="1" t="str">
+      <c r="D5" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6">
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11">
         <v>500</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="11">
         <f>50</f>
         <v>50</v>
       </c>
-      <c r="M5" s="1" t="e">
+      <c r="M5" s="10" t="e">
         <f>10^((LOG(AVERAGE(I5:J5)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K5</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N5" s="1" t="e">
+      <c r="N5" s="10" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O5" s="1"/>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B6" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B6" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C6" s="2" t="str">
+      <c r="C6" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D6" s="1" t="str">
+      <c r="D6" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6">
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11">
         <v>500</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="11">
         <f>50</f>
         <v>50</v>
       </c>
-      <c r="M6" s="1" t="e">
+      <c r="M6" s="10" t="e">
         <f>10^((LOG(AVERAGE(I6:J6)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K6</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N6" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O6" s="1"/>
+      <c r="N6" s="10" t="e">
+        <f>(L6/10^3 * M6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B7" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B7" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C7" s="2" t="str">
+      <c r="C7" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D7" s="1" t="str">
+      <c r="D7" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6">
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11">
         <v>500</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="11">
         <f>50</f>
         <v>50</v>
       </c>
-      <c r="M7" s="1" t="e">
+      <c r="M7" s="10" t="e">
         <f>10^((LOG(AVERAGE(I7:J7)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K7</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" s="1" t="e">
+      <c r="N7" s="10" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O7" s="1"/>
+      <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B8" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B8" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C8" s="5" t="str">
+      <c r="C8" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D8" s="4" t="str">
+      <c r="D8" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7">
-        <v>16</v>
-      </c>
-      <c r="L8" s="7">
-        <v>100</v>
-      </c>
-      <c r="M8" s="4" t="e">
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4">
+        <v>500</v>
+      </c>
+      <c r="L8" s="4">
+        <f>50</f>
+        <v>50</v>
+      </c>
+      <c r="M8" s="1" t="e">
         <f>10^((LOG(AVERAGE(I8:J8)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K8</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N8" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O8" t="e">
-        <f t="shared" ref="O8:O13" si="2">N8/(N2+N8+N14) * 100</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="N8" s="1" t="e">
+        <f t="shared" ref="N8:N10" si="2">(L8/10^3 * M8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B9" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B9" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C9" s="5" t="str">
+      <c r="C9" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D9" s="4" t="str">
+      <c r="D9" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7">
-        <v>16</v>
-      </c>
-      <c r="L9" s="7">
-        <v>100</v>
-      </c>
-      <c r="M9" s="4" t="e">
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
+        <v>500</v>
+      </c>
+      <c r="L9" s="4">
+        <f>50</f>
+        <v>50</v>
+      </c>
+      <c r="M9" s="1" t="e">
         <f>10^((LOG(AVERAGE(I9:J9)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O9" t="e">
+      <c r="N9" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="O9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B10" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B10" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C10" s="5" t="str">
+      <c r="C10" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D10" s="4" t="str">
+      <c r="D10" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7">
-        <v>16</v>
-      </c>
-      <c r="L10" s="7">
-        <v>100</v>
-      </c>
-      <c r="M10" s="4" t="e">
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4">
+        <v>500</v>
+      </c>
+      <c r="L10" s="4">
+        <f>50</f>
+        <v>50</v>
+      </c>
+      <c r="M10" s="1" t="e">
         <f>10^((LOG(AVERAGE(I10:J10)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K10</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O10" t="e">
+      <c r="N10" s="1" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B11" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B11" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C11" s="5" t="str">
+      <c r="C11" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D11" s="4" t="str">
+      <c r="D11" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5">
         <v>16</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="5">
         <v>100</v>
       </c>
-      <c r="M11" s="4" t="e">
+      <c r="M11" s="3" t="e">
         <f>10^((LOG(AVERAGE(I11:J11)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K11</f>
         <v>#DIV/0!</v>
       </c>
@@ -3068,48 +3725,48 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O11" t="e">
-        <f t="shared" si="2"/>
+        <f>N11/(N2+N11+N20) * 100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B12" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B12" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C12" s="5" t="str">
+      <c r="C12" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D12" s="4" t="str">
+      <c r="D12" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5">
         <v>16</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="5">
         <v>100</v>
       </c>
-      <c r="M12" s="4" t="e">
+      <c r="M12" s="3" t="e">
         <f>10^((LOG(AVERAGE(I12:J12)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K12</f>
         <v>#DIV/0!</v>
       </c>
@@ -3118,48 +3775,48 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O12" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="O12:O19" si="3">N12/(N3+N12+N21) * 100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B13" s="5" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B13" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C13" s="5" t="str">
+      <c r="C13" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D13" s="4" t="str">
+      <c r="D13" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7">
+        <v>5</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5">
         <v>16</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="5">
         <v>100</v>
       </c>
-      <c r="M13" s="4" t="e">
+      <c r="M13" s="3" t="e">
         <f>10^((LOG(AVERAGE(I13:J13)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K13</f>
         <v>#DIV/0!</v>
       </c>
@@ -3168,307 +3825,757 @@
         <v>#DIV/0!</v>
       </c>
       <c r="O13" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B14" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B14" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C14" s="2" t="str">
+      <c r="C14" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D14" s="1" t="str">
+      <c r="D14" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6">
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11">
         <v>16</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="11">
         <v>100</v>
       </c>
-      <c r="M14" s="1" t="e">
+      <c r="M14" s="10" t="e">
         <f>10^((LOG(AVERAGE(I14:J14)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K14</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N14" s="1" t="e">
+      <c r="N14" s="10" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O14" s="1" t="e">
-        <f t="shared" ref="O14:O19" si="3">N14/(N2+N14) * 100</f>
+      <c r="O14" s="10" t="e">
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B15" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B15" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C15" s="2" t="str">
+      <c r="C15" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D15" s="1" t="str">
+      <c r="D15" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6">
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11">
         <v>16</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="11">
         <v>100</v>
       </c>
-      <c r="M15" s="1" t="e">
+      <c r="M15" s="10" t="e">
         <f>10^((LOG(AVERAGE(I15:J15)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K15</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N15" s="1" t="e">
+      <c r="N15" s="10" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O15" s="1" t="e">
+      <c r="O15" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B16" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B16" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C16" s="2" t="str">
+      <c r="C16" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D16" s="1" t="str">
+      <c r="D16" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6">
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11">
         <v>16</v>
       </c>
-      <c r="L16" s="6">
+      <c r="L16" s="11">
         <v>100</v>
       </c>
-      <c r="M16" s="1" t="e">
+      <c r="M16" s="10" t="e">
         <f>10^((LOG(AVERAGE(I16:J16)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K16</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N16" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="1" t="e">
+      <c r="N16" s="10" t="e">
+        <f>(L16/10^3 * M16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="10" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B17" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B17" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C17" s="2" t="str">
+      <c r="C17" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D17" s="1" t="str">
+      <c r="D17" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="6" t="s">
+      <c r="E17" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6">
+      <c r="F17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5">
         <v>16</v>
       </c>
-      <c r="L17" s="6">
+      <c r="L17" s="5">
         <v>100</v>
       </c>
-      <c r="M17" s="1" t="e">
+      <c r="M17" s="3" t="e">
         <f>10^((LOG(AVERAGE(I17:J17)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N17" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="1" t="e">
+      <c r="N17" t="e">
+        <f t="shared" ref="N17:N19" si="4">(L17/10^3 * M17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B18" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B18" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C18" s="2" t="str">
+      <c r="C18" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D18" s="1" t="str">
+      <c r="D18" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="6" t="s">
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6">
+      <c r="F18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5">
         <v>16</v>
       </c>
-      <c r="L18" s="6">
+      <c r="L18" s="5">
         <v>100</v>
       </c>
-      <c r="M18" s="1" t="e">
+      <c r="M18" s="3" t="e">
         <f>10^((LOG(AVERAGE(I18:J18)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N18" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O18" s="1" t="e">
+      <c r="N18" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="15">
         <f ca="1">Blank!A$2</f>
-        <v>43839</v>
-      </c>
-      <c r="B19" s="2" t="str">
+        <v>43892</v>
+      </c>
+      <c r="B19" s="15" t="str">
         <f>Blank!B$2</f>
         <v>You</v>
       </c>
-      <c r="C19" s="2" t="str">
+      <c r="C19" s="15" t="str">
         <f>Blank!C$2</f>
         <v>PROJECT_NAME</v>
       </c>
-      <c r="D19" s="1" t="str">
+      <c r="D19" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>NAME</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5">
+        <v>16</v>
+      </c>
+      <c r="L19" s="5">
+        <v>100</v>
+      </c>
+      <c r="M19" s="3" t="e">
+        <f>10^((LOG(AVERAGE(I19:J19)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B20" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C20" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D20" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4">
+        <v>16</v>
+      </c>
+      <c r="L20" s="4">
+        <v>100</v>
+      </c>
+      <c r="M20" s="1" t="e">
+        <f>10^((LOG(AVERAGE(I20:J20)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K20</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" s="1" t="e">
+        <f>N20/(N2+N20) * 100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B21" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C21" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D21" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4">
+        <v>16</v>
+      </c>
+      <c r="L21" s="4">
+        <v>100</v>
+      </c>
+      <c r="M21" s="1" t="e">
+        <f>10^((LOG(AVERAGE(I21:J21)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" s="1" t="e">
+        <f t="shared" ref="O21:O28" si="5">N21/(N3+N21) * 100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B22" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C22" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D22" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4">
+        <v>16</v>
+      </c>
+      <c r="L22" s="4">
+        <v>100</v>
+      </c>
+      <c r="M22" s="1" t="e">
+        <f>10^((LOG(AVERAGE(I22:J22)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B23" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C23" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D23" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6">
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11">
         <v>16</v>
       </c>
-      <c r="L19" s="6">
+      <c r="L23" s="11">
         <v>100</v>
       </c>
-      <c r="M19" s="1" t="e">
-        <f>10^((LOG(AVERAGE(I19:J19)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K19</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" s="1" t="e">
+      <c r="M23" s="10" t="e">
+        <f>10^((LOG(AVERAGE(I23:J23)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K23</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" s="10" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O19" s="1" t="e">
-        <f t="shared" si="3"/>
+      <c r="O23" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B24" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C24" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D24" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11">
+        <v>16</v>
+      </c>
+      <c r="L24" s="11">
+        <v>100</v>
+      </c>
+      <c r="M24" s="10" t="e">
+        <f>10^((LOG(AVERAGE(I24:J24)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K24</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N24" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O24" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B25" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C25" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D25" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11">
+        <v>16</v>
+      </c>
+      <c r="L25" s="11">
+        <v>100</v>
+      </c>
+      <c r="M25" s="10" t="e">
+        <f>10^((LOG(AVERAGE(I25:J25)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K25</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" s="10" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" s="10" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B26" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C26" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D26" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4">
+        <v>16</v>
+      </c>
+      <c r="L26" s="4">
+        <v>100</v>
+      </c>
+      <c r="M26" s="1" t="e">
+        <f>10^((LOG(AVERAGE(I26:J26)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K26</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N26" s="1" t="e">
+        <f t="shared" ref="N26:N28" si="6">(L26/10^3 * M26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O26" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B27" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C27" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D27" s="16" t="str">
+        <f ca="1">RIGHT(CELL("nomfichier",A26),LEN(CELL("nomfichier",A26))-SEARCH("]",CELL("nomfichier",A26)))</f>
+        <v>NAME</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4">
+        <v>16</v>
+      </c>
+      <c r="L27" s="4">
+        <v>100</v>
+      </c>
+      <c r="M27" s="1" t="e">
+        <f>10^((LOG(AVERAGE(I27:J27)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N27" s="1" t="e">
+        <f>(L27/10^3 * M27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O27" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <f ca="1">Blank!A$2</f>
+        <v>43892</v>
+      </c>
+      <c r="B28" s="15" t="str">
+        <f>Blank!B$2</f>
+        <v>You</v>
+      </c>
+      <c r="C28" s="15" t="str">
+        <f>Blank!C$2</f>
+        <v>PROJECT_NAME</v>
+      </c>
+      <c r="D28" s="16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>NAME</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4">
+        <v>16</v>
+      </c>
+      <c r="L28" s="4">
+        <v>100</v>
+      </c>
+      <c r="M28" s="1" t="e">
+        <f>10^((LOG(AVERAGE(I28:J28)-Blank!$H$2, 10)-Blank!$M$2)/Blank!$N$2) * K28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N28" s="1" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O28" s="1" t="e">
+        <f>N28/(N10+N28) * 100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3476,5 +4583,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>